<commit_message>
Hanh thêm pipeline.md chưa thống nhất, chỉ đang dự kiến
</commit_message>
<xml_diff>
--- a/PhanTichNguLieu.xlsx
+++ b/PhanTichNguLieu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIT 3rd year\CS212\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C4FDEC-378D-45C7-BEAF-022F4AF4502E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E304F937-4899-467C-BD44-E97C541C268A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A650E3B7-C1A8-4E3A-8287-E070FCF1FC10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="115">
   <si>
     <t>Label</t>
   </si>
@@ -281,27 +281,6 @@
   </si>
   <si>
     <t>Đây là 1 bình luận mang nghĩa tiêu cực được thể hiện qua việc người dùng nêu rằng "bỏ đánh dấu không hẹn ngày gọi ship tiếp" đồng thời có mô tả lý do là "k có một cục sườn nào chứ đừng nói sụn gì" với giá là "98k". Chữ "k" ở cụm "k có một cục sườn…" mang nghĩa là "không" còn "k" ở "98k" là "ngàn" mô tả mệnh giá tiền.</t>
-  </si>
-  <si>
-    <t>giới thiệu bài toán</t>
-  </si>
-  <si>
-    <t>quá trình thu thập dữ liệu</t>
-  </si>
-  <si>
-    <t>kết quả phân tích ngữ liệu, điểm cần chú ý</t>
-  </si>
-  <si>
-    <t>Phương pháp sử dụng</t>
-  </si>
-  <si>
-    <t>kết quả, ví dụ hiệu quả chạy qua câu ví dụ</t>
-  </si>
-  <si>
-    <t>Kết quả đánh giá trên tập dữ liệu, các mô hình dùng để so sánh (tên, setting, kết quả không cần nói kỹ)</t>
-  </si>
-  <si>
-    <t>Nhận xét kết quả mô hình của mình, đúng/sai, vì sao</t>
   </si>
   <si>
     <t>Nội dung của bình luận này chứa cả yếu tố tích cực lẫn tiêu cực. Trong đó, có phần tích cực thông qua v iệc khen cháo có "vị đặc trưng thơm mùi gạo mùi thịt", "rất mê", "ăn mê người", "no đẫy bụng",  "sẽ quay lại", "tuyệt vờiiiiiii". Bên cạnh đó cũng có phần tiêu cực là "hơi bị mặn" nhưng chỉ là thỉnh thoảng và câu đầu tiên "chả bao giờ muốn ăn hàng cháo ở ngõ Huyện"  thì hàng cháo này chưa xác định rõ là hàng cháo nào khác hay hàng cháo đang xét. Tuy nhiên về mặt tổng thể rõ ràng bình luận này mang tính tích cực và việc gán nhãn tiêu cực là không hợp lý.</t>
@@ -571,9 +550,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,6 +557,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1359419E-551A-4708-9270-F87DA8AAC2D3}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1120,21 +1099,21 @@
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1148,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1162,7 +1141,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="70" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="70" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f>A4+1</f>
         <v>2</v>
@@ -1176,11 +1155,8 @@
       <c r="D5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" ht="70" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" ref="A6:A53" si="0">A5+1</f>
         <v>3</v>
@@ -1194,11 +1170,8 @@
       <c r="D6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" ht="70" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1212,11 +1185,8 @@
       <c r="D7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="154" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" ht="154" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1230,11 +1200,8 @@
       <c r="D8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="56" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1248,11 +1215,8 @@
       <c r="D9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" ht="70" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1266,29 +1230,23 @@
       <c r="D10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="112" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+    </row>
+    <row r="11" spans="1:4" ht="112" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="84" x14ac:dyDescent="0.3">
+      <c r="D11" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="84" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1300,10 +1258,10 @@
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="70" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1315,10 +1273,10 @@
         <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="56" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="56" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1330,10 +1288,10 @@
         <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="98" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="98" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1345,22 +1303,22 @@
         <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="70" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="70" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>76</v>
+      <c r="D16" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1375,7 +1333,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="56" x14ac:dyDescent="0.3">
@@ -1390,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1405,7 +1363,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1420,7 +1378,7 @@
         <v>20</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="56" x14ac:dyDescent="0.3">
@@ -1435,7 +1393,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1450,7 +1408,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1465,7 +1423,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="210" x14ac:dyDescent="0.3">
@@ -1480,7 +1438,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="98" x14ac:dyDescent="0.3">
@@ -1495,7 +1453,7 @@
         <v>25</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1510,7 +1468,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="98" x14ac:dyDescent="0.3">
@@ -1525,7 +1483,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1540,7 +1498,7 @@
         <v>28</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="140" x14ac:dyDescent="0.3">
@@ -1555,7 +1513,7 @@
         <v>30</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="84" x14ac:dyDescent="0.3">
@@ -1570,7 +1528,7 @@
         <v>31</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1585,7 +1543,7 @@
         <v>32</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1600,7 +1558,7 @@
         <v>33</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1615,7 +1573,7 @@
         <v>34</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="210" x14ac:dyDescent="0.3">
@@ -1630,7 +1588,7 @@
         <v>35</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="84" x14ac:dyDescent="0.3">
@@ -1645,7 +1603,7 @@
         <v>36</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1660,7 +1618,7 @@
         <v>37</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1675,7 +1633,7 @@
         <v>38</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1690,7 +1648,7 @@
         <v>39</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="56" x14ac:dyDescent="0.3">
@@ -1705,7 +1663,7 @@
         <v>40</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1720,7 +1678,7 @@
         <v>41</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="56" x14ac:dyDescent="0.3">
@@ -1735,7 +1693,7 @@
         <v>42</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1750,7 +1708,7 @@
         <v>43</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1765,7 +1723,7 @@
         <v>44</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="56" x14ac:dyDescent="0.3">
@@ -1780,7 +1738,7 @@
         <v>45</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="70" x14ac:dyDescent="0.3">
@@ -1795,7 +1753,7 @@
         <v>46</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="84" x14ac:dyDescent="0.3">
@@ -1810,7 +1768,7 @@
         <v>47</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="56" x14ac:dyDescent="0.3">
@@ -1825,7 +1783,7 @@
         <v>48</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="308" x14ac:dyDescent="0.3">
@@ -1840,7 +1798,7 @@
         <v>49</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -1855,7 +1813,7 @@
         <v>50</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="98" x14ac:dyDescent="0.3">
@@ -1870,7 +1828,7 @@
         <v>51</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="210" x14ac:dyDescent="0.3">
@@ -1885,7 +1843,7 @@
         <v>52</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="196" x14ac:dyDescent="0.3">
@@ -1900,7 +1858,7 @@
         <v>53</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="210" x14ac:dyDescent="0.3">
@@ -1915,7 +1873,7 @@
         <v>54</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,43 +1886,43 @@
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:4" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="C57" s="11" t="s">
-        <v>119</v>
+      <c r="C57" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="C59" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="C61" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="56" x14ac:dyDescent="0.3">
       <c r="C62" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="70" x14ac:dyDescent="0.3">
       <c r="C63" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="28" x14ac:dyDescent="0.3">
       <c r="C64" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>